<commit_message>
updated pin spreadsheet planner for 3sonar
</commit_message>
<xml_diff>
--- a/spreadsheets/rp2-pin-planner-artcar-3sonar.xlsx
+++ b/spreadsheets/rp2-pin-planner-artcar-3sonar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradcarlile/Documents/GitHub/artcar-ultrasonic-dist-rp2/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1B35FD-D56F-DB4D-93D4-D3042A6971A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC210EFC-DE1D-AE4F-9173-F6E017332781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7460" yWindow="-21100" windowWidth="24520" windowHeight="20120" xr2:uid="{9994E188-9327-AB46-AF3F-8738237FB097}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="92">
   <si>
     <t>gp0</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>&lt;any unused pin&gt;</t>
+  </si>
+  <si>
+    <t>? Rotary encoder?</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -679,29 +682,26 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1047,8 +1047,8 @@
   </sheetPr>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="111" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1068,12 +1068,12 @@
       <c r="A1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
       <c r="G1" t="s">
         <v>85</v>
       </c>
@@ -1167,13 +1167,13 @@
       <c r="A10" s="7">
         <v>2</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="34" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="19" t="s">
@@ -1190,24 +1190,22 @@
       <c r="A11" s="7">
         <v>3</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
       <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>4</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="20"/>
@@ -1225,13 +1223,13 @@
       <c r="A13" s="7">
         <v>5</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="34" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="20"/>
@@ -1249,13 +1247,13 @@
       <c r="A14" s="7">
         <v>6</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="34" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="19" t="s">
@@ -1275,13 +1273,13 @@
       <c r="A15" s="7">
         <v>7</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="34" t="s">
         <v>43</v>
       </c>
       <c r="E15" s="19" t="s">
@@ -1301,71 +1299,78 @@
       <c r="A16" s="7">
         <v>8</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>9</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="20"/>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>10</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="34" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="20"/>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>11</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="34" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>12</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="34" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="19" t="s">
@@ -1382,24 +1387,22 @@
       <c r="A21" s="7">
         <v>13</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
       <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>14</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="20"/>
@@ -1417,13 +1420,13 @@
       <c r="A23" s="7">
         <v>15</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="34" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="20"/>
@@ -1441,13 +1444,13 @@
       <c r="A24" s="7">
         <v>16</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="34" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="19" t="s">
@@ -1467,13 +1470,13 @@
       <c r="A25" s="7">
         <v>17</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="34" t="s">
         <v>43</v>
       </c>
       <c r="E25" s="19" t="s">
@@ -1493,24 +1496,22 @@
       <c r="A26" s="7">
         <v>18</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
       <c r="E26" s="20"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>19</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="20"/>
@@ -1572,10 +1573,10 @@
       <c r="B31" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="34" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="19" t="s">
@@ -1598,8 +1599,6 @@
       <c r="B32" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
       <c r="E32" s="20"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1609,10 +1608,10 @@
       <c r="B33" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E33" s="20"/>
@@ -1633,10 +1632,10 @@
       <c r="B34" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="34" t="s">
         <v>45</v>
       </c>
       <c r="E34" s="20"/>
@@ -1657,8 +1656,7 @@
       <c r="B35" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="36" t="s">
+      <c r="D35" s="34" t="s">
         <v>42</v>
       </c>
       <c r="E35" s="20"/>
@@ -1679,8 +1677,7 @@
       <c r="B36" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="34" t="s">
         <v>43</v>
       </c>
       <c r="E36" s="20"/>
@@ -1701,8 +1698,6 @@
       <c r="B37" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
       <c r="E37" s="20"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1712,8 +1707,6 @@
       <c r="B38" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
       <c r="E38" s="20"/>
       <c r="G38" t="s">
         <v>87</v>
@@ -1729,8 +1722,6 @@
       <c r="B39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
       <c r="E39" s="20"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1740,10 +1731,10 @@
       <c r="B40" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E40" s="20"/>
@@ -1764,10 +1755,10 @@
       <c r="B41" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="36" t="s">
+      <c r="D41" s="34" t="s">
         <v>45</v>
       </c>
       <c r="E41" s="20"/>
@@ -1789,10 +1780,9 @@
       <c r="B42" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="38"/>
       <c r="E42" s="20"/>
       <c r="G42" t="s">
         <v>88</v>
@@ -1805,10 +1795,9 @@
       <c r="B43" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="38"/>
       <c r="E43" s="20"/>
       <c r="G43" t="s">
         <v>89</v>
@@ -1822,10 +1811,9 @@
         <v>35</v>
       </c>
       <c r="B44" s="7"/>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="38"/>
       <c r="E44" s="20"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1835,8 +1823,6 @@
       <c r="B45" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
       <c r="E45" s="20"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -1846,8 +1832,6 @@
       <c r="B46" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
       <c r="E46" s="20"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -1857,9 +1841,10 @@
       <c r="B47" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
       <c r="E47" s="20"/>
+      <c r="G47" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -1868,8 +1853,6 @@
       <c r="B48" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
       <c r="E48" s="20"/>
     </row>
     <row r="49" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>